<commit_message>
Complet Arm State and Adding Item State
</commit_message>
<xml_diff>
--- a/Framework_DX11/Client/Bin/DataFiles/Item_Initialize_Data.xlsx
+++ b/Framework_DX11/Client/Bin/DataFiles/Item_Initialize_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeamProject\Bulid\NewBulid_12_02\Dx11_LiesOfP\Framework_DX11\Client\Bin\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C8DFDED-35FC-4FB4-ABEE-0400CE81EE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED2C9215-D54D-408A-B1DB-CF48D37E7A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1310,7 +1310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1318,6 +1318,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1600,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1723,7 +1724,7 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="str">
+      <c r="B9" s="7" t="str">
         <f>VLOOKUP(C9,Sheet2!$A:$B,2)</f>
         <v>그라인더</v>
       </c>
@@ -1738,7 +1739,7 @@
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="str">
+      <c r="B10" s="7" t="str">
         <f>VLOOKUP(C10,Sheet2!$A:$B,2)</f>
         <v>문페이즈 회중시계</v>
       </c>
@@ -1768,7 +1769,7 @@
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="str">
+      <c r="B12" s="7" t="str">
         <f>VLOOKUP(C12,Sheet2!$A:$B,2)</f>
         <v>테르밋</v>
       </c>
@@ -1798,7 +1799,7 @@
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="str">
+      <c r="B14" s="7" t="str">
         <f>VLOOKUP(C14,Sheet2!$A:$B,2)</f>
         <v>펄스전지</v>
       </c>
@@ -2098,7 +2099,7 @@
       <c r="A34">
         <v>31</v>
       </c>
-      <c r="B34" s="6" t="str">
+      <c r="B34" s="7" t="str">
         <f>VLOOKUP(C34,Sheet2!$A:$B,2)</f>
         <v>최후의 수단</v>
       </c>
@@ -2308,7 +2309,7 @@
       <c r="A48">
         <v>45</v>
       </c>
-      <c r="B48" s="6" t="str">
+      <c r="B48" s="7" t="str">
         <f>VLOOKUP(C48,Sheet2!$A:$B,2)</f>
         <v>속성 정화 앰플</v>
       </c>
@@ -2473,10 +2474,10 @@
         <v>4</v>
       </c>
       <c r="C59" s="3">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3">
         <v>1</v>
-      </c>
-      <c r="D59" s="3">
-        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2487,10 +2488,10 @@
         <v>5</v>
       </c>
       <c r="C60" s="3">
+        <v>0</v>
+      </c>
+      <c r="D60" s="3">
         <v>2</v>
-      </c>
-      <c r="D60" s="3">
-        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2501,10 +2502,10 @@
         <v>6</v>
       </c>
       <c r="C61" s="3">
+        <v>2</v>
+      </c>
+      <c r="D61" s="3">
         <v>0</v>
-      </c>
-      <c r="D61" s="3">
-        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2518,7 +2519,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2529,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="C63" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2546,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="D64" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2560,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="D65" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2574,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="D66" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2588,7 +2589,7 @@
         <v>2</v>
       </c>
       <c r="D67" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>